<commit_message>
Stable version 1.55 - various bugfixes & optimization work (SAP Connectors etc.)
</commit_message>
<xml_diff>
--- a/default_parameters.xlsx
+++ b/default_parameters.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ludwig\OneDrive - UiPath\Studio - Projects\Own Demos\1 - Document_Understanding\SSD-SAPSUperDemo 1.44\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ludwig\OneDrive - UiPath\Studio - Projects\Own Demos\1 - Document_Understanding\SSD-SAPSUperDemo WIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6CCCAC-5C93-4F9E-B997-1F349797AA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A56B3E3-B0E3-464C-AC9F-8A08CCF32E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15375" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="other_param" sheetId="3" r:id="rId2"/>
-    <sheet name="dir_structure" sheetId="1" r:id="rId3"/>
+    <sheet name="I2S_other_param" sheetId="3" r:id="rId2"/>
+    <sheet name="I2S_dir_structure" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="editable" localSheetId="1">other_param!$B$3:$B$3</definedName>
-    <definedName name="editable">dir_structure!$B$2:$C$5</definedName>
+    <definedName name="editable" localSheetId="1">I2S_other_param!$B$3:$B$3</definedName>
+    <definedName name="editable">I2S_dir_structure!$B$2:$C$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -198,7 +198,7 @@
     <t>YES</t>
   </si>
   <si>
-    <t>Value</t>
+    <t>Default-Value</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
         <v>32</v>
       </c>
       <c r="B4" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -777,7 +777,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
-    <protectedRange sqref="B2:B3" name="Range1"/>
+    <protectedRange sqref="B2:B9" name="Range1"/>
   </protectedRanges>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" xr:uid="{FD52B01E-41DE-419E-BAC6-E219EABDF63D}"/>
@@ -792,7 +792,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- Fixed annoying Excel date format - added more config settings - generalized the config settings
</commit_message>
<xml_diff>
--- a/default_parameters.xlsx
+++ b/default_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefan.reutter\Documents\UiPath\SharedDemos\SSD-SAPSuperDemo_Stable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Demos\uipath-invoice2sap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5909F81-7EDD-49C4-AE7B-B1CB8A924213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D102BDEA-2791-460B-83FE-88ABC8747F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Explanation</t>
   </si>
@@ -114,18 +114,12 @@
     <t>mail_folder</t>
   </si>
   <si>
-    <t>Inbox\SAPDemo</t>
-  </si>
-  <si>
     <t>Mailbox where the Invoices should be found</t>
   </si>
   <si>
     <t>SAP_username</t>
   </si>
   <si>
-    <t>S4H_FIN</t>
-  </si>
-  <si>
     <t>Usernname for SAP_Logon</t>
   </si>
   <si>
@@ -156,9 +150,6 @@
     <t>mail_sendto</t>
   </si>
   <si>
-    <t>ludwig.wilhelm@uipath.com</t>
-  </si>
-  <si>
     <t>Default email if choosen to send results</t>
   </si>
   <si>
@@ -180,18 +171,9 @@
     <t>asset_orch_folder</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>which folder is the asset (see above) located in Orchestrator?</t>
   </si>
   <si>
-    <t>asset_orch_Login</t>
-  </si>
-  <si>
-    <t>SAP_Login</t>
-  </si>
-  <si>
     <t>the name of the Orchestrator Asset</t>
   </si>
   <si>
@@ -199,6 +181,54 @@
   </si>
   <si>
     <t>Default-Value</t>
+  </si>
+  <si>
+    <t>DSF_2976</t>
+  </si>
+  <si>
+    <t>Inbox\Invoice2SAP</t>
+  </si>
+  <si>
+    <t>meganb@M365x018209.onmicrosoft.com</t>
+  </si>
+  <si>
+    <t>DSF_SAPLogin</t>
+  </si>
+  <si>
+    <t>DSF_sreutter001_uipath</t>
+  </si>
+  <si>
+    <t>use_validation_station</t>
+  </si>
+  <si>
+    <t>Should the validation station be used?</t>
+  </si>
+  <si>
+    <t>enter_in_sap</t>
+  </si>
+  <si>
+    <t>Enter invoice into SAP?</t>
+  </si>
+  <si>
+    <t>display_form</t>
+  </si>
+  <si>
+    <t>Display the form for settings?</t>
+  </si>
+  <si>
+    <t>Send result log to the above e-mail address?</t>
+  </si>
+  <si>
+    <t>mail_results</t>
+  </si>
+  <si>
+    <t>display_animation</t>
+  </si>
+  <si>
+    <t>Display on-screen messages about the robot status</t>
+  </si>
+  <si>
+    <t>asset_orch_login</t>
   </si>
 </sst>
 </file>
@@ -635,10 +665,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F8CA9D-B5A4-40B3-A07B-6CF965121D2C}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -653,27 +683,27 @@
         <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.5">
@@ -681,105 +711,175 @@
         <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="4" t="b">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="4">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
         <v>37</v>
-      </c>
-      <c r="B7" s="4" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="B8" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>41</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="B2:B9" name="Range1"/>
+    <protectedRange sqref="B2:B13" name="Range1"/>
   </protectedRanges>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{FD52B01E-41DE-419E-BAC6-E219EABDF63D}"/>
+    <hyperlink ref="B6" r:id="rId1" display="ludwig.wilhelm@uipath.com" xr:uid="{FD52B01E-41DE-419E-BAC6-E219EABDF63D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -817,7 +917,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.5">
@@ -825,7 +925,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1</v>
@@ -834,7 +934,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.5">
@@ -842,7 +942,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>2</v>
@@ -851,7 +951,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.5">
@@ -859,7 +959,7 @@
         <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -868,7 +968,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
@@ -876,7 +976,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
@@ -885,7 +985,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>